<commit_message>
Yapay verilerde başarı sağlandı. Gerçek veriler için son kontrol yapılacak. Cep kontrolü yapılacak.
</commit_message>
<xml_diff>
--- a/FuzzyMsc/App_Data/Tmp/FileUploads/yapay-veriler-2.xlsx
+++ b/FuzzyMsc/App_Data/Tmp/FileUploads/yapay-veriler-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="REZISTIVITE" sheetId="1" r:id="rId1"/>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +563,7 @@
         <v>70</v>
       </c>
       <c r="G3" s="1">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1">
         <v>250</v>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>

</xml_diff>